<commit_message>
compiling filings into one excel
</commit_message>
<xml_diff>
--- a/input/Financial Statement GPS/IncomeStatements-GPS.xlsx
+++ b/input/Financial Statement GPS/IncomeStatements-GPS.xlsx
@@ -7,25 +7,29 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Year Ended 2017" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Q2 2018 (2017)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Q3 2018 (2017)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Year Ended 2018" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Q2 2019 (2018)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Q3 2019 (2018)" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Year Ended 2019" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Q1 2020 (2019)" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Q2 2020 (2019)" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Q3 2020 (2019)" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Year Ended 2020" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Q2 2021 (2020)" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Q3 2021 (2020)" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Year Ended 2021" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Q1 2022 (2021)" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Q2 2022 (2021)" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Q3 2022 (2021)" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Year Ended 2022" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Q1 2023 (2022)" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Q2 2017 (2016)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Q3 2017 (2016)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Year Ended 2017" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Q2 2018 (2017)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Q3 2018 (2017)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Year Ended 2018" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Q1 2019 (2018)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Q2 2019 (2018)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Q3 2019 (2018)" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Year Ended 2019" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Q1 2020 (2019)" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Q2 2020 (2019)" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Q3 2020 (2019)" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Year Ended 2020" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Q1 2021 (2020)" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Q2 2021 (2020)" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Q3 2021 (2020)" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Year Ended 2021" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Q1 2022 (2021)" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Q2 2022 (2021)" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Q3 2022 (2021)" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Year Ended 2022" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Q1 2023 (2022)" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +463,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan. 28, 2017</t>
+          <t>Jul. 30, 2016</t>
         </is>
       </c>
     </row>
@@ -470,7 +474,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15516</v>
+        <v>3851</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +484,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9876</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +494,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5640</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="5">
@@ -500,7 +504,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4449</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +514,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1191</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +524,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -530,7 +534,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9">
@@ -540,7 +544,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1124</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10">
@@ -550,7 +554,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>448</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11">
@@ -560,17 +564,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>676</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13">
@@ -580,7 +584,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +594,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.69</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="15">
@@ -600,7 +604,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.69</v>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
@@ -630,18 +644,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nov. 02, 2019</t>
+          <t>Feb. 02, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net Sales</t>
+          <t>Revenues</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3998</v>
+        <v>16580</v>
       </c>
     </row>
     <row r="3">
@@ -651,7 +665,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2439</v>
+        <v>10258</v>
       </c>
     </row>
     <row r="4">
@@ -661,17 +675,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1559</v>
+        <v>6322</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1338</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="6">
@@ -681,17 +695,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>221</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
@@ -701,7 +715,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-7</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="9">
@@ -711,7 +725,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>209</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="10">
@@ -721,7 +735,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>69</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11">
@@ -731,17 +745,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>140</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13">
@@ -751,7 +765,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14">
@@ -761,7 +775,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.37</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="15">
@@ -771,17 +785,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.37</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+          <t>Common Stock, Dividends, Per Share, Declared</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -811,18 +825,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 01, 2020</t>
+          <t>May 04, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16383</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="3">
@@ -832,7 +846,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10250</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="4">
@@ -842,17 +856,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6133</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5559</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6">
@@ -862,17 +876,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>574</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -882,7 +896,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-30</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="9">
@@ -892,7 +906,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>528</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10">
@@ -902,7 +916,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>177</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -912,17 +926,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>351</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13">
@@ -932,7 +946,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14">
@@ -942,7 +956,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.93</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15">
@@ -952,17 +966,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.93</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Common Stock, Dividends, Per Share, Declared</t>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.97</v>
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -976,7 +990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -992,76 +1006,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 01, 2020</t>
+          <t>Aug. 03, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-62</v>
+        <v>4005</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2449</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-10</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $(1), $1, $1, and $5</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-8</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $(3), $(1), and $(5)</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-6</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-86</v>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Income before income taxes</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Net income</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Earnings per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -1075,7 +1171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1091,96 +1187,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Oct. 31, 2020</t>
+          <t>Nov. 02, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2439</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $-, $-, $1, and $5</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-2</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $-, $(2), and $(5)</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+          <t>Income before income taxes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+          <t>Income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Net income</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Earnings per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1368,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan. 30, 2021</t>
+          <t>Feb. 01, 2020</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1379,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13800000000</v>
+        <v>16383</v>
       </c>
     </row>
     <row r="3">
@@ -1231,7 +1389,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9095000000</v>
+        <v>10250</v>
       </c>
     </row>
     <row r="4">
@@ -1241,7 +1399,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4705000000</v>
+        <v>6133</v>
       </c>
     </row>
     <row r="5">
@@ -1251,117 +1409,117 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5567000000</v>
+        <v>5559</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Operating income (loss)</t>
+          <t>Operating income</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-862000000</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Gain (Loss) on Extinguishment of Debt</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58000000</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>192000000</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Interest income</t>
+          <t>Income before income taxes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-10000000</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Income (loss) before income taxes</t>
+          <t>Income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1102000000</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Income taxes</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-437000000</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-665000000</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - diluted (in shares)</t>
+          <t>Earnings per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>374</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Earnings per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.78</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Common Stock, Dividends, Per Share, Declared</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.78</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -1370,6 +1528,204 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>May 02, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-932</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Foreign currency translation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax of $2 and $4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $- and $(2)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-926</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Aug. 01, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Foreign currency translation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax of $(1), $1, $1, and $5</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $(3), $(1), and $(5)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1391,7 +1747,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 01, 2021</t>
+          <t>Oct. 31, 2020</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1758,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
@@ -1420,27 +1776,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $- and $2</t>
+          <t>Change in fair value of derivative financial instruments, net of tax of $-, $-, $1, and $5</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-7</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $- and $-</t>
+          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $-, $(2), and $(5)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7">
@@ -1450,7 +1806,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1460,7 +1816,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>159</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
@@ -1480,225 +1836,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Jul. 31, 2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Net income (loss)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Foreign currency translation</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for losses (gains) on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Oct. 30, 2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Net income (loss)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-152</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Foreign currency translation</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-144</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1728,18 +1866,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan. 29, 2022</t>
+          <t>Jan. 30, 2021</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net sales</t>
+          <t>Revenues</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16670000000</v>
+        <v>13800000000</v>
       </c>
     </row>
     <row r="3">
@@ -1749,7 +1887,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10033000000</v>
+        <v>9095000000</v>
       </c>
     </row>
     <row r="4">
@@ -1759,7 +1897,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6637000000</v>
+        <v>4705000000</v>
       </c>
     </row>
     <row r="5">
@@ -1769,7 +1907,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5827000000</v>
+        <v>5567000000</v>
       </c>
     </row>
     <row r="6">
@@ -1779,17 +1917,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>810000000</v>
+        <v>-862000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Loss on extinguishment of debt</t>
+          <t>Gain (Loss) on Extinguishment of Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>325000000</v>
+        <v>58000000</v>
       </c>
     </row>
     <row r="8">
@@ -1799,7 +1937,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>167000000</v>
+        <v>192000000</v>
       </c>
     </row>
     <row r="9">
@@ -1809,7 +1947,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-5000000</v>
+        <v>-10000000</v>
       </c>
     </row>
     <row r="10">
@@ -1819,7 +1957,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>323000000</v>
+        <v>-1102000000</v>
       </c>
     </row>
     <row r="11">
@@ -1829,7 +1967,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>67000000</v>
+        <v>-437000000</v>
       </c>
     </row>
     <row r="12">
@@ -1839,47 +1977,47 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>256000000</v>
+        <v>-665000000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—diluted</t>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings (loss) per share—basic</t>
+          <t>Earnings per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.68</v>
+        <v>-1.78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Earnings (loss) per share—diluted</t>
+          <t>Earnings per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.67</v>
+        <v>-1.78</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +2031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1909,7 +2047,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Apr. 30, 2022</t>
+          <t>May 01, 2021</t>
         </is>
       </c>
     </row>
@@ -1920,7 +2058,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3">
@@ -1938,27 +2076,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+          <t>Change in fair value of derivative financial instruments, net of tax of $- and $2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $- and $-</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -1968,7 +2106,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="8">
@@ -1978,7 +2116,27 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-154</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +2166,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jul. 29, 2017</t>
+          <t>Oct. 29, 2016</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2177,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3799</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="3">
@@ -2029,7 +2187,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2320</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="4">
@@ -2039,7 +2197,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1479</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="5">
@@ -2049,7 +2207,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1028</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="6">
@@ -2059,7 +2217,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>451</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7">
@@ -2069,7 +2227,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -2079,7 +2237,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="9">
@@ -2089,7 +2247,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>439</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10">
@@ -2109,7 +2267,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>271</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12">
@@ -2119,7 +2277,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13">
@@ -2129,7 +2287,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
@@ -2139,7 +2297,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="15">
@@ -2149,7 +2307,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.68</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="16">
@@ -2167,7 +2325,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jul. 31, 2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Foreign currency translation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for losses (gains) on derivative financial instruments, net of (tax) tax benefit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Oct. 30, 2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Foreign currency translation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2189,7 +2565,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Oct. 28, 2017</t>
+          <t>Jan. 29, 2022</t>
         </is>
       </c>
     </row>
@@ -2200,7 +2576,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3838</v>
+        <v>16670000000</v>
       </c>
     </row>
     <row r="3">
@@ -2210,7 +2586,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2313</v>
+        <v>10033000000</v>
       </c>
     </row>
     <row r="4">
@@ -2220,7 +2596,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1525</v>
+        <v>6637000000</v>
       </c>
     </row>
     <row r="5">
@@ -2230,117 +2606,117 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1147</v>
+        <v>5827000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Operating income</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>378</v>
+        <v>810000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Loss on extinguishment of debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>325000000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Interest income</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-4</v>
+        <v>167000000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Income before income taxes</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>364</v>
+        <v>-5000000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Income taxes</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>135</v>
+        <v>323000000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Net income</t>
+          <t>Income taxes</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>229</v>
+        <v>67000000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Net income (loss)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>391</v>
+        <v>256000000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - diluted (in shares)</t>
+          <t>Weighted-average number of shares—basic</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>393</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Weighted-average number of shares—diluted</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.59</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Earnings (loss) per share—basic</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.58</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+          <t>Earnings (loss) per share—diluted</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.23</v>
+        <v>0.67</v>
       </c>
     </row>
   </sheetData>
@@ -2348,7 +2724,106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Apr. 30, 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-162</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Foreign currency translation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other comprehensive income (loss), net of tax</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2370,7 +2845,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 03, 2018</t>
+          <t>Jan. 28, 2017</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2856,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15855</v>
+        <v>15516</v>
       </c>
     </row>
     <row r="3">
@@ -2391,7 +2866,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9789</v>
+        <v>9876</v>
       </c>
     </row>
     <row r="4">
@@ -2401,7 +2876,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6066</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="5">
@@ -2411,7 +2886,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4587</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="6">
@@ -2421,7 +2896,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1479</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="7">
@@ -2431,7 +2906,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -2441,7 +2916,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-19</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="9">
@@ -2451,7 +2926,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1424</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="10">
@@ -2461,7 +2936,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>576</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11">
@@ -2471,7 +2946,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>848</v>
+        <v>676</v>
       </c>
     </row>
     <row r="12">
@@ -2481,7 +2956,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13">
@@ -2491,7 +2966,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
@@ -2501,7 +2976,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.16</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="15">
@@ -2511,7 +2986,188 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.14</v>
+        <v>1.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jul. 29, 2017</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net sales</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gross profit</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Operating expenses</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Operating income</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Interest expense</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Interest income</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Income before income taxes</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Net income</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Earnings per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
@@ -2541,18 +3197,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 04, 2018</t>
+          <t>Oct. 28, 2017</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net Sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4085</v>
+        <v>3838</v>
       </c>
     </row>
     <row r="3">
@@ -2562,7 +3218,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2458</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="4">
@@ -2572,17 +3228,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1627</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1229</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="6">
@@ -2592,17 +3248,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>398</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -2612,7 +3268,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-7</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="9">
@@ -2622,7 +3278,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10">
@@ -2632,7 +3288,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>91</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11">
@@ -2642,7 +3298,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>297</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12">
@@ -2652,7 +3308,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13">
@@ -2662,7 +3318,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14">
@@ -2672,7 +3328,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.77</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="15">
@@ -2682,7 +3338,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.76</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="16">
@@ -2692,7 +3348,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +3362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2722,18 +3378,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nov. 03, 2018</t>
+          <t>Feb. 03, 2018</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net Sales</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4089</v>
+        <v>15855</v>
       </c>
     </row>
     <row r="3">
@@ -2743,7 +3399,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2466</v>
+        <v>9789</v>
       </c>
     </row>
     <row r="4">
@@ -2753,17 +3409,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1623</v>
+        <v>6066</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1260</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="6">
@@ -2773,17 +3429,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>363</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
@@ -2793,7 +3449,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="9">
@@ -2803,7 +3459,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>350</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="10">
@@ -2813,7 +3469,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>84</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11">
@@ -2823,17 +3479,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>266</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13">
@@ -2843,7 +3499,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14">
@@ -2853,7 +3509,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6899999999999999</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="15">
@@ -2863,17 +3519,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>2.14</v>
       </c>
     </row>
   </sheetData>
@@ -2903,18 +3549,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 02, 2019</t>
+          <t>May 05, 2018</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues</t>
+          <t>Net sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16580</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="3">
@@ -2924,7 +3570,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10258</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="4">
@@ -2934,17 +3580,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6322</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4960</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="6">
@@ -2954,17 +3600,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1362</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -2974,7 +3620,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-33</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="9">
@@ -2984,7 +3630,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1322</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
@@ -2994,7 +3640,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>319</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -3004,17 +3650,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1003</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13">
@@ -3024,7 +3670,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14">
@@ -3034,7 +3680,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.61</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="15">
@@ -3044,17 +3690,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.59</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Common Stock, Dividends, Per Share, Declared</t>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.97</v>
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -3084,7 +3730,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 04, 2019</t>
+          <t>Aug. 04, 2018</t>
         </is>
       </c>
     </row>
@@ -3095,7 +3741,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3706</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="3">
@@ -3105,7 +3751,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2362</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="4">
@@ -3115,7 +3761,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1344</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="5">
@@ -3125,7 +3771,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1028</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="6">
@@ -3135,7 +3781,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>316</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
@@ -3145,7 +3791,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -3155,7 +3801,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9">
@@ -3165,7 +3811,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>302</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10">
@@ -3175,7 +3821,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11">
@@ -3185,7 +3831,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>227</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12">
@@ -3195,7 +3841,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13">
@@ -3205,7 +3851,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
@@ -3215,7 +3861,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="15">
@@ -3225,7 +3871,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="16">
@@ -3265,7 +3911,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 03, 2019</t>
+          <t>Nov. 03, 2018</t>
         </is>
       </c>
     </row>
@@ -3276,7 +3922,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4005</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="3">
@@ -3286,7 +3932,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2449</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="4">
@@ -3296,7 +3942,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1556</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="5">
@@ -3306,7 +3952,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1274</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="6">
@@ -3316,7 +3962,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>282</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7">
@@ -3326,7 +3972,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -3346,7 +3992,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>271</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10">
@@ -3356,7 +4002,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
@@ -3366,7 +4012,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>168</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12">
@@ -3376,7 +4022,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13">
@@ -3386,7 +4032,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14">
@@ -3396,7 +4042,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.44</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -3406,7 +4052,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.44</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
work on income to match up and minimize rows
</commit_message>
<xml_diff>
--- a/input/Financial Statement GPS/IncomeStatements-GPS.xlsx
+++ b/input/Financial Statement GPS/IncomeStatements-GPS.xlsx
@@ -7,29 +7,27 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Q2 2017 (2016)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Q3 2017 (2016)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Year Ended 2017" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Q2 2018 (2017)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Q3 2018 (2017)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Year Ended 2018" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Q1 2019 (2018)" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Q2 2019 (2018)" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Q3 2019 (2018)" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Year Ended 2019" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Q1 2020 (2019)" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Q2 2020 (2019)" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Q3 2020 (2019)" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Year Ended 2020" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Q1 2021 (2020)" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Q2 2021 (2020)" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Q3 2021 (2020)" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Year Ended 2021" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Q1 2022 (2021)" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Q2 2022 (2021)" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Q3 2022 (2021)" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Year Ended 2022" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Q1 2023 (2022)" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Year Ended 2017" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Q2 2018 (2017)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Q3 2018 (2017)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Year Ended 2018" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Q1 2019 (2018)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Q2 2019 (2018)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Q3 2019 (2018)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Year Ended 2019" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Q1 2020 (2019)" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Q2 2020 (2019)" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Q3 2020 (2019)" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Year Ended 2020" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Q1 2021 (2020)" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Q2 2021 (2020)" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Q3 2021 (2020)" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Year Ended 2021" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Q1 2022 (2021)" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Q2 2022 (2021)" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Q3 2022 (2021)" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Year Ended 2022" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Q1 2023 (2022)" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +461,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jul. 30, 2016</t>
+          <t>Jan. 28, 2017</t>
         </is>
       </c>
     </row>
@@ -474,7 +472,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3851</v>
+        <v>15516</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +482,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2414</v>
+        <v>9876</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +492,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1437</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="5">
@@ -504,7 +502,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1158</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="6">
@@ -514,7 +512,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>279</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="7">
@@ -524,7 +522,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +532,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="9">
@@ -544,7 +542,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>263</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="10">
@@ -554,7 +552,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>138</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11">
@@ -564,17 +562,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>125</v>
+        <v>676</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13">
@@ -584,7 +582,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
@@ -594,7 +592,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.31</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="15">
@@ -604,17 +602,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.23</v>
+        <v>1.69</v>
       </c>
     </row>
   </sheetData>
@@ -644,18 +632,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 02, 2019</t>
+          <t>Aug. 03, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16580</v>
+        <v>4005</v>
       </c>
     </row>
     <row r="3">
@@ -665,7 +653,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10258</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="4">
@@ -675,17 +663,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6322</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4960</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="6">
@@ -695,17 +683,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1362</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -715,7 +703,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-33</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +713,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1322</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10">
@@ -735,7 +723,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>319</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11">
@@ -745,17 +733,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1003</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13">
@@ -765,7 +753,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14">
@@ -775,7 +763,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.61</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="15">
@@ -785,17 +773,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.59</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Common Stock, Dividends, Per Share, Declared</t>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.97</v>
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +813,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 04, 2019</t>
+          <t>Nov. 02, 2019</t>
         </is>
       </c>
     </row>
@@ -836,7 +824,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3706</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="3">
@@ -846,7 +834,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2362</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="4">
@@ -856,7 +844,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1344</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="5">
@@ -866,7 +854,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1028</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="6">
@@ -876,7 +864,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>316</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
@@ -886,7 +874,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -896,7 +884,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9">
@@ -906,7 +894,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>302</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
@@ -916,7 +904,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
@@ -926,7 +914,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>227</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
@@ -936,7 +924,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13">
@@ -946,7 +934,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14">
@@ -956,7 +944,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="15">
@@ -966,7 +954,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="16">
@@ -1006,18 +994,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 03, 2019</t>
+          <t>Feb. 01, 2020</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net Sales</t>
+          <t>Revenues</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4005</v>
+        <v>16383</v>
       </c>
     </row>
     <row r="3">
@@ -1027,7 +1015,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2449</v>
+        <v>10250</v>
       </c>
     </row>
     <row r="4">
@@ -1037,17 +1025,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1556</v>
+        <v>6133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1274</v>
+        <v>5559</v>
       </c>
     </row>
     <row r="6">
@@ -1057,17 +1045,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>282</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -1077,7 +1065,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="9">
@@ -1087,7 +1075,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>271</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10">
@@ -1097,7 +1085,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>103</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
@@ -1107,17 +1095,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>168</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13">
@@ -1127,7 +1115,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14">
@@ -1137,7 +1125,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.44</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="15">
@@ -1147,17 +1135,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.44</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+          <t>Common Stock, Dividends, Per Share, Declared</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -1171,7 +1159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,7 +1175,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nov. 02, 2019</t>
+          <t>May 02, 2020</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1186,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3998</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="3">
@@ -1208,7 +1196,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2439</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="4">
@@ -1218,7 +1206,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1559</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5">
@@ -1228,17 +1216,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1338</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Operating income</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>221</v>
+        <v>-1244</v>
       </c>
     </row>
     <row r="7">
@@ -1258,17 +1246,17 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-7</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Income before income taxes</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>209</v>
+        <v>-1259</v>
       </c>
     </row>
     <row r="10">
@@ -1278,17 +1266,17 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>69</v>
+        <v>-327</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Net income</t>
+          <t>Net income (loss)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>140</v>
+        <v>-932</v>
       </c>
     </row>
     <row r="12">
@@ -1298,7 +1286,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13">
@@ -1308,37 +1296,27 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.37</v>
+        <v>-2.51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>-2.51</v>
       </c>
     </row>
   </sheetData>
@@ -1368,18 +1346,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 01, 2020</t>
+          <t>Aug. 01, 2020</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16383</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="3">
@@ -1389,7 +1367,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10250</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="4">
@@ -1399,127 +1377,127 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6133</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5559</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Operating income</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>574</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Gain (Loss) on Extinguishment of Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Interest income</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Income before income taxes</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>528</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Income taxes</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>177</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Net income</t>
+          <t>Income taxes</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>351</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Net income (loss)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>376</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - diluted (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.93</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.93</v>
+        <v>-0.17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Common Stock, Dividends, Per Share, Declared</t>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.97</v>
+        <v>-0.17</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1549,76 +1527,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 02, 2020</t>
+          <t>Oct. 31, 2020</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-932</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2374</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-9</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $2 and $4</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $- and $(2)</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-4</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Gain (Loss) on Extinguishment of Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-926</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Interest income</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Income (loss) before income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1648,76 +1708,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 01, 2020</t>
+          <t>Jan. 30, 2021</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Revenues</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-62</v>
+        <v>13800000000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9095000000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-10</v>
+        <v>4705000000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $(1), $1, $1, and $5</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-8</v>
+        <v>5567000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $(3), $(1), and $(5)</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-6</v>
+        <v>-862000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Gain (Loss) on Extinguishment of Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-24</v>
+        <v>58000000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-86</v>
+        <v>192000000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Interest income</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Income (loss) before income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1102000000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-437000000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-665000000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares—basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-1.78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Earnings per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.78</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1747,96 +1889,148 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Oct. 31, 2020</t>
+          <t>May 01, 2021</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2361</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $-, $-, $1, and $5</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-2</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $(1), $-, $(2), and $(5)</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+          <t>Income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.43</v>
       </c>
     </row>
   </sheetData>
@@ -1866,18 +2060,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan. 30, 2021</t>
+          <t>Jul. 31, 2021</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13800000000</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="3">
@@ -1887,7 +2081,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9095000000</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="4">
@@ -1897,17 +2091,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4705000000</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5567000000</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="6">
@@ -1917,7 +2111,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-862000000</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7">
@@ -1927,17 +2121,17 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>192000000</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
@@ -1947,7 +2141,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-10000000</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10">
@@ -1957,7 +2151,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1102000000</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11">
@@ -1967,7 +2161,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-437000000</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
@@ -1977,17 +2171,17 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-665000000</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14">
@@ -1997,27 +2191,27 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.78</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.78</v>
+        <v>0.67</v>
       </c>
     </row>
   </sheetData>
@@ -2031,7 +2225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,96 +2241,158 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 01, 2021</t>
+          <t>Oct. 30, 2021</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net income (loss)</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>166</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2282</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foreign currency translation</t>
+          <t>Gross profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax of $- and $2</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-7</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for gains on derivative financial instruments, net of tax of $- and $-</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other comprehensive income (loss), net of tax</t>
+          <t>Gain (Loss) on Extinguishment of Debt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-7</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Comprehensive income (loss)</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>159</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
+          <t>Interest income</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>-215</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Net income (loss)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +2422,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Oct. 29, 2016</t>
+          <t>Jul. 29, 2017</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2433,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3798</v>
+        <v>3799</v>
       </c>
     </row>
     <row r="3">
@@ -2187,7 +2443,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2305</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="4">
@@ -2197,7 +2453,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1493</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="5">
@@ -2207,7 +2463,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1104</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6">
@@ -2217,7 +2473,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>389</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7">
@@ -2227,7 +2483,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2493,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="9">
@@ -2247,7 +2503,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>372</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10">
@@ -2267,7 +2523,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>204</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12">
@@ -2277,7 +2533,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13">
@@ -2287,7 +2543,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14">
@@ -2297,7 +2553,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.51</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -2307,7 +2563,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.51</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="16">
@@ -2326,224 +2582,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Jul. 31, 2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Net income (loss)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Foreign currency translation</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for losses (gains) on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Oct. 30, 2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Net income (loss)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-152</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Foreign currency translation</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-144</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2724,106 +2762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Apr. 30, 2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Net income (loss)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-162</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Foreign currency translation</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Change in fair value of derivative financial instruments, net of tax (tax benefit)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Reclassification adjustment for (gains) losses on derivative financial instruments, net of (tax) tax benefit</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Other comprehensive income (loss), net of tax</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2845,18 +2784,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan. 28, 2017</t>
+          <t>Apr. 30, 2022</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net sales</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15516</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="3">
@@ -2866,7 +2805,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9876</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="4">
@@ -2876,37 +2815,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5640</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4449</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Operating income</t>
+          <t>Operating income (loss)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1191</v>
+        <v>-197</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -2916,17 +2855,17 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Income before income taxes</t>
+          <t>Income (loss) before income taxes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1124</v>
+        <v>-216</v>
       </c>
     </row>
     <row r="10">
@@ -2936,27 +2875,27 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>448</v>
+        <v>-54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Net income</t>
+          <t>Net income (loss)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>676</v>
+        <v>-162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>399</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13">
@@ -2966,27 +2905,27 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>400</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Earnings per share - basic (in dollars per share)</t>
+          <t>Earnings (loss) per share - basic (in dollars per share)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.69</v>
+        <v>-0.44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Earnings per share - diluted (in dollars per share)</t>
+          <t>Earnings (loss) per share - diluted (in dollars per share)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.69</v>
+        <v>-0.44</v>
       </c>
     </row>
   </sheetData>
@@ -2994,7 +2933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3016,7 +2955,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jul. 29, 2017</t>
+          <t>Oct. 28, 2017</t>
         </is>
       </c>
     </row>
@@ -3027,7 +2966,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3799</v>
+        <v>3838</v>
       </c>
     </row>
     <row r="3">
@@ -3037,7 +2976,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2320</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="4">
@@ -3047,7 +2986,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1479</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="5">
@@ -3057,7 +2996,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1028</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="6">
@@ -3067,7 +3006,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>451</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7">
@@ -3077,7 +3016,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -3097,7 +3036,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>439</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10">
@@ -3107,7 +3046,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11">
@@ -3117,7 +3056,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>271</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12">
@@ -3127,7 +3066,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13">
@@ -3137,7 +3076,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14">
@@ -3147,7 +3086,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="15">
@@ -3157,7 +3096,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.68</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="16">
@@ -3168,6 +3107,177 @@
       </c>
       <c r="B16" t="n">
         <v>0.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Feb. 03, 2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Net sales</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15855</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cost of goods sold and occupancy expenses</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9789</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gross profit</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>6066</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Operating expenses</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Operating income</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Interest expense</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Interest income</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Income before income taxes</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Net income</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares—basic (in shares)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weighted-average number of shares - diluted (in shares)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Earnings per share - basic (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Earnings per share - diluted (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2.14</v>
       </c>
     </row>
   </sheetData>
@@ -3197,7 +3307,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Oct. 28, 2017</t>
+          <t>May 05, 2018</t>
         </is>
       </c>
     </row>
@@ -3208,7 +3318,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3838</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="3">
@@ -3218,7 +3328,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2313</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="4">
@@ -3228,17 +3338,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1525</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1147</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="6">
@@ -3248,17 +3358,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>378</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -3268,7 +3378,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-4</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="9">
@@ -3278,7 +3388,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>364</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
@@ -3288,7 +3398,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>135</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -3298,7 +3408,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>229</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12">
@@ -3308,7 +3418,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13">
@@ -3328,7 +3438,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.59</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="15">
@@ -3338,7 +3448,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.58</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="16">
@@ -3348,7 +3458,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.23</v>
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -3362,7 +3472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3378,18 +3488,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Feb. 03, 2018</t>
+          <t>Aug. 04, 2018</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net sales</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15855</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="3">
@@ -3399,7 +3509,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9789</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="4">
@@ -3409,17 +3519,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6066</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating expenses</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4587</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="6">
@@ -3429,17 +3539,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1479</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest expense</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -3449,7 +3559,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-19</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9">
@@ -3459,7 +3569,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1424</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10">
@@ -3469,7 +3579,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>576</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11">
@@ -3479,17 +3589,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>848</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares—basic (in shares)</t>
+          <t>Weighted-average number of shares - basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13">
@@ -3499,7 +3609,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
@@ -3509,7 +3619,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.16</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="15">
@@ -3519,7 +3629,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.14</v>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2425</v>
       </c>
     </row>
   </sheetData>
@@ -3549,18 +3669,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>May 05, 2018</t>
+          <t>Nov. 03, 2018</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net sales</t>
+          <t>Net Sales</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3783</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="3">
@@ -3570,7 +3690,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2356</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="4">
@@ -3580,7 +3700,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1427</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="5">
@@ -3590,7 +3710,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1198</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="6">
@@ -3600,7 +3720,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>229</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7">
@@ -3610,7 +3730,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -3620,7 +3740,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="9">
@@ -3630,7 +3750,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>219</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10">
@@ -3640,7 +3760,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
@@ -3650,7 +3770,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>164</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12">
@@ -3660,7 +3780,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13">
@@ -3670,7 +3790,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14">
@@ -3680,7 +3800,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.42</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -3690,7 +3810,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.42</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -3730,18 +3850,18 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Aug. 04, 2018</t>
+          <t>Feb. 02, 2019</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Net Sales</t>
+          <t>Revenues</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4085</v>
+        <v>16580</v>
       </c>
     </row>
     <row r="3">
@@ -3751,7 +3871,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2458</v>
+        <v>10258</v>
       </c>
     </row>
     <row r="4">
@@ -3761,17 +3881,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1627</v>
+        <v>6322</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Operating expenses</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1229</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="6">
@@ -3781,17 +3901,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>398</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Interest expense</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
@@ -3801,7 +3921,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-7</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="9">
@@ -3811,7 +3931,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>388</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="10">
@@ -3821,7 +3941,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>91</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11">
@@ -3831,17 +3951,17 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>297</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Weighted-average number of shares - basic (in shares)</t>
+          <t>Weighted-average number of shares—basic (in shares)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13">
@@ -3851,7 +3971,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14">
@@ -3861,7 +3981,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.77</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="15">
@@ -3871,17 +3991,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.76</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cash dividends declared and paid per share (in dollars per share)</t>
+          <t>Common Stock, Dividends, Per Share, Declared</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2425</v>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +4031,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nov. 03, 2018</t>
+          <t>May 04, 2019</t>
         </is>
       </c>
     </row>
@@ -3922,7 +4042,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4089</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="3">
@@ -3932,7 +4052,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2466</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="4">
@@ -3942,7 +4062,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1623</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="5">
@@ -3952,7 +4072,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1260</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6">
@@ -3962,7 +4082,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>363</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7">
@@ -3972,7 +4092,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -3982,7 +4102,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="9">
@@ -3992,7 +4112,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>350</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10">
@@ -4002,7 +4122,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -4012,7 +4132,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>266</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12">
@@ -4022,7 +4142,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13">
@@ -4032,7 +4152,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14">
@@ -4042,7 +4162,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15">
@@ -4052,7 +4172,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16">

</xml_diff>